<commit_message>
open file functionality and calculation part added
</commit_message>
<xml_diff>
--- a/Demo from test.xlsx
+++ b/Demo from test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Research\Detector Software\V3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Research\Developed softwares\Detector Software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63285866-29F4-4A9A-80BC-9DCD34D9295F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3695D5E3-15A7-4683-B7A8-BFDD373A4931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>Z-Scan Sample analysis had done at SSN Research Center on 10 Jul 2024 22:04:40</t>
   </si>
@@ -202,9 +202,6 @@
     <t>5 mm</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>Open Aperture</t>
   </si>
   <si>
@@ -217,9 +214,6 @@
     <t>Close Aperture</t>
   </si>
   <si>
-    <t>20 %</t>
-  </si>
-  <si>
     <t>Transmitance</t>
   </si>
   <si>
@@ -242,6 +236,9 @@
   </si>
   <si>
     <t>4.5 mm</t>
+  </si>
+  <si>
+    <t>85 %</t>
   </si>
 </sst>
 </file>
@@ -322,12 +319,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -640,7 +637,7 @@
   <dimension ref="A1:G139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,155 +646,176 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
+      <c r="B2" s="5"/>
       <c r="C2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="5"/>
       <c r="C3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="5"/>
       <c r="C4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="4"/>
+      <c r="B5" s="5"/>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="5"/>
+      <c r="B6" s="6"/>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="4"/>
+      <c r="B7" s="5"/>
       <c r="C7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="4"/>
+      <c r="B8" s="5"/>
       <c r="C8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="5"/>
-      <c r="C9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="5"/>
-      <c r="C10" t="s">
-        <v>29</v>
+      <c r="D10">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="4"/>
+      <c r="B11" s="5"/>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" t="s">
-        <v>16</v>
+      <c r="B12" s="6"/>
+      <c r="C12" s="3">
+        <v>1.8</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="3" t="s">
-        <v>21</v>
+        <v>28</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>26</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="6"/>
+      <c r="A17" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="7"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="C18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -2496,11 +2514,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A17:B17"/>
@@ -2512,6 +2525,11 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>